<commit_message>
gen yaml for table fk refer
</commit_message>
<xml_diff>
--- a/data/name/cn.family.v1.xlsx
+++ b/data/name/cn.family.v1.xlsx
@@ -1,24 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEA749C-A46B-A449-88F0-7613C56ADD76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB55864-DE5C-D346-813D-C16F969669C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="1940" windowWidth="20940" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2000" yWindow="2500" windowWidth="20940" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="中文姓" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -4689,7 +4681,7 @@
   <dimension ref="A1:D1075"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="14"/>
@@ -19751,7 +19743,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C1945">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C1945">
     <sortCondition ref="B2:B1945"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>